<commit_message>
Tyche GUI dev code
</commit_message>
<xml_diff>
--- a/src/technology/tutorial-basic/tutorial-basic.xlsx
+++ b/src/technology/tutorial-basic/tutorial-basic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\tyche\src\technology\tutorial-basic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nrel-my.sharepoint.com/personal/tghosh_nrel_gov/Documents/work_NREL/tyche/src/technology/tutorial-basic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E468CA5-93EA-4819-88FC-470ADA17A9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{0E468CA5-93EA-4819-88FC-470ADA17A9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61DEFD93-BE62-EB4D-963B-2A763A47F036}"/>
   <bookViews>
-    <workbookView xWindow="30990" yWindow="345" windowWidth="17730" windowHeight="15120" xr2:uid="{AA06EC71-7717-4C82-8350-2B72D254338B}"/>
+    <workbookView xWindow="14280" yWindow="4900" windowWidth="17740" windowHeight="15120" activeTab="1" xr2:uid="{AA06EC71-7717-4C82-8350-2B72D254338B}"/>
   </bookViews>
   <sheets>
     <sheet name="designs" sheetId="1" r:id="rId1"/>
@@ -716,21 +716,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D58172A-44BA-47D6-958C-3833F35637FC}">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -753,7 +753,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -776,7 +776,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -799,7 +799,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -822,7 +822,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -845,7 +845,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -868,7 +868,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -891,7 +891,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -914,7 +914,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -937,7 +937,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -960,7 +960,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -983,7 +983,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>6</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>6</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>6</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>6</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>6</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>6</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>6</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>6</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>6</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>6</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>6</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>6</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>6</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>6</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>6</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>6</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>6</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>6</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>6</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>6</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>6</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>6</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>6</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>6</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>6</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>6</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>6</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>6</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>6</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>6</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>6</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>6</v>
       </c>
@@ -2731,7 +2731,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>6</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>6</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>6</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>6</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>6</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>6</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>6</v>
       </c>
@@ -2892,7 +2892,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>6</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>6</v>
       </c>
@@ -2938,7 +2938,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>6</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>6</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>6</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>6</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>6</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>6</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>6</v>
       </c>
@@ -3099,7 +3099,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>6</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>6</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>6</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>6</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>6</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>6</v>
       </c>
@@ -3237,7 +3237,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>6</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>6</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>6</v>
       </c>
@@ -3306,7 +3306,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>6</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>6</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>6</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>6</v>
       </c>
@@ -3398,7 +3398,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>6</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>6</v>
       </c>
@@ -3444,7 +3444,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>6</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>6</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>6</v>
       </c>
@@ -3522,11 +3522,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DBA2671-2D19-4EE1-92E2-838007A235E3}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="33.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3552,9 +3558,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
         <v>49</v>
@@ -3586,9 +3592,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3608,7 +3614,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3625,7 +3631,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3642,7 +3648,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -3659,7 +3665,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -3676,7 +3682,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -3693,7 +3699,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -3710,7 +3716,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3727,7 +3733,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -3744,7 +3750,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -3761,7 +3767,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -3791,14 +3797,14 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -3812,7 +3818,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -3823,7 +3829,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -3834,7 +3840,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>76</v>
       </c>
@@ -3858,18 +3864,18 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="59" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3892,7 +3898,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3915,7 +3921,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3938,7 +3944,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -3961,7 +3967,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -3984,7 +3990,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -4007,7 +4013,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -4030,7 +4036,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -4053,7 +4059,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -4076,7 +4082,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -4099,7 +4105,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -4122,7 +4128,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -4145,7 +4151,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -4168,7 +4174,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -4191,7 +4197,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -4214,7 +4220,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -4237,7 +4243,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -4260,7 +4266,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -4283,7 +4289,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -4306,7 +4312,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -4329,7 +4335,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -4352,7 +4358,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -4375,7 +4381,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -4398,7 +4404,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -4421,7 +4427,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -4444,7 +4450,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -4467,7 +4473,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -4490,7 +4496,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -4513,7 +4519,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -4536,7 +4542,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -4559,7 +4565,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -4582,7 +4588,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -4605,7 +4611,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -4628,7 +4634,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -4651,7 +4657,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -4674,7 +4680,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -4697,7 +4703,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -4720,7 +4726,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -4743,7 +4749,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -4766,7 +4772,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -4789,7 +4795,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -4812,7 +4818,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -4835,7 +4841,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -4858,7 +4864,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -4881,7 +4887,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -4904,7 +4910,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>6</v>
       </c>
@@ -4927,7 +4933,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -4950,7 +4956,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -4973,7 +4979,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -4996,7 +5002,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -5019,7 +5025,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>6</v>
       </c>
@@ -5042,7 +5048,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>6</v>
       </c>
@@ -5065,7 +5071,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -5088,7 +5094,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -5111,7 +5117,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -5134,7 +5140,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -5157,7 +5163,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -5180,7 +5186,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -5203,7 +5209,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>6</v>
       </c>
@@ -5226,7 +5232,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>6</v>
       </c>
@@ -5249,7 +5255,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>6</v>
       </c>
@@ -5283,9 +5289,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5302,7 +5308,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -5316,7 +5322,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -5330,7 +5336,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -5344,7 +5350,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -5358,7 +5364,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -5372,7 +5378,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -5399,14 +5405,14 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -5420,7 +5426,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -5431,7 +5437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -5442,7 +5448,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -5453,7 +5459,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -5464,7 +5470,7 @@
         <v>9000000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -5475,7 +5481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -5486,7 +5492,7 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>78</v>
       </c>
@@ -5497,7 +5503,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -5508,7 +5514,7 @@
         <v>7000000</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -5519,7 +5525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>79</v>
       </c>
@@ -5530,7 +5536,7 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>79</v>
       </c>
@@ -5541,7 +5547,7 @@
         <v>4000000</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>79</v>
       </c>

</xml_diff>

<commit_message>
Linking GUI with Tyche
</commit_message>
<xml_diff>
--- a/src/technology/tutorial-basic/tutorial-basic.xlsx
+++ b/src/technology/tutorial-basic/tutorial-basic.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nrel-my.sharepoint.com/personal/tghosh_nrel_gov/Documents/work_NREL/tyche/src/technology/tutorial-basic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{0E468CA5-93EA-4819-88FC-470ADA17A9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61DEFD93-BE62-EB4D-963B-2A763A47F036}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{0E468CA5-93EA-4819-88FC-470ADA17A9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29F4DA6A-9AA1-CF45-BDB2-01A5D63F5BEA}"/>
   <bookViews>
     <workbookView xWindow="14280" yWindow="4900" windowWidth="17740" windowHeight="15120" activeTab="1" xr2:uid="{AA06EC71-7717-4C82-8350-2B72D254338B}"/>
   </bookViews>
@@ -3523,7 +3523,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3560,7 +3560,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Updates to technologies json and generation of technologies json file.
</commit_message>
<xml_diff>
--- a/src/technology/tutorial-basic/tutorial-basic.xlsx
+++ b/src/technology/tutorial-basic/tutorial-basic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\tyche\src\technology\tutorial-basic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nrel-my.sharepoint.com/personal/tghosh_nrel_gov/Documents/work_NREL/tyche/tyche/src/technology/tutorial-basic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E468CA5-93EA-4819-88FC-470ADA17A9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{0E468CA5-93EA-4819-88FC-470ADA17A9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0C94348-6077-134A-ADA5-AB285B98840C}"/>
   <bookViews>
-    <workbookView xWindow="30990" yWindow="345" windowWidth="17730" windowHeight="15120" xr2:uid="{AA06EC71-7717-4C82-8350-2B72D254338B}"/>
+    <workbookView xWindow="38240" yWindow="3300" windowWidth="17740" windowHeight="15120" activeTab="6" xr2:uid="{AA06EC71-7717-4C82-8350-2B72D254338B}"/>
   </bookViews>
   <sheets>
     <sheet name="designs" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="110">
   <si>
     <t>Technology</t>
   </si>
@@ -363,6 +363,15 @@
   </si>
   <si>
     <t>Tower Reference</t>
+  </si>
+  <si>
+    <t>Investment in Drive only</t>
+  </si>
+  <si>
+    <t>Investment in Tower only</t>
+  </si>
+  <si>
+    <t>Investment in Rotor only</t>
   </si>
 </sst>
 </file>
@@ -716,21 +725,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D58172A-44BA-47D6-958C-3833F35637FC}">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A94" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -753,7 +762,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -776,7 +785,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -799,7 +808,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -822,7 +831,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -845,7 +854,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -868,7 +877,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -891,7 +900,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -914,7 +923,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -937,7 +946,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -960,7 +969,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -983,7 +992,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1006,7 +1015,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1029,7 +1038,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1052,7 +1061,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1075,7 +1084,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1098,7 +1107,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1121,7 +1130,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1144,7 +1153,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1167,7 +1176,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1190,7 +1199,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1213,7 +1222,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -1236,7 +1245,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -1259,7 +1268,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1282,7 +1291,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1305,7 +1314,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1328,7 +1337,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -1351,7 +1360,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1374,7 +1383,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -1397,7 +1406,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1420,7 +1429,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -1443,7 +1452,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -1466,7 +1475,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -1489,7 +1498,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -1512,7 +1521,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -1535,7 +1544,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -1558,7 +1567,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -1581,7 +1590,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -1604,7 +1613,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -1627,7 +1636,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -1650,7 +1659,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -1673,7 +1682,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -1696,7 +1705,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -1719,7 +1728,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -1742,7 +1751,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -1765,7 +1774,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>6</v>
       </c>
@@ -1788,7 +1797,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -1811,7 +1820,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -1834,7 +1843,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -1857,7 +1866,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -1880,7 +1889,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>6</v>
       </c>
@@ -1903,7 +1912,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>6</v>
       </c>
@@ -1926,7 +1935,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -1949,7 +1958,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -1972,7 +1981,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -1995,7 +2004,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -2018,7 +2027,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -2041,7 +2050,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -2064,7 +2073,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>6</v>
       </c>
@@ -2087,7 +2096,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>6</v>
       </c>
@@ -2110,7 +2119,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>6</v>
       </c>
@@ -2133,7 +2142,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>6</v>
       </c>
@@ -2156,7 +2165,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>6</v>
       </c>
@@ -2179,7 +2188,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>6</v>
       </c>
@@ -2202,7 +2211,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>6</v>
       </c>
@@ -2225,7 +2234,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>6</v>
       </c>
@@ -2248,7 +2257,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>6</v>
       </c>
@@ -2271,7 +2280,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>6</v>
       </c>
@@ -2294,7 +2303,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>6</v>
       </c>
@@ -2317,7 +2326,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>6</v>
       </c>
@@ -2340,7 +2349,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>6</v>
       </c>
@@ -2363,7 +2372,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>6</v>
       </c>
@@ -2386,7 +2395,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>6</v>
       </c>
@@ -2409,7 +2418,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>6</v>
       </c>
@@ -2432,7 +2441,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>6</v>
       </c>
@@ -2455,7 +2464,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>6</v>
       </c>
@@ -2478,7 +2487,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>6</v>
       </c>
@@ -2501,7 +2510,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>6</v>
       </c>
@@ -2524,7 +2533,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>6</v>
       </c>
@@ -2547,7 +2556,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>6</v>
       </c>
@@ -2570,7 +2579,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>6</v>
       </c>
@@ -2593,7 +2602,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>6</v>
       </c>
@@ -2616,7 +2625,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>6</v>
       </c>
@@ -2639,7 +2648,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>6</v>
       </c>
@@ -2662,7 +2671,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>6</v>
       </c>
@@ -2685,7 +2694,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>6</v>
       </c>
@@ -2708,7 +2717,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>6</v>
       </c>
@@ -2731,7 +2740,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>6</v>
       </c>
@@ -2754,7 +2763,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>6</v>
       </c>
@@ -2777,7 +2786,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>6</v>
       </c>
@@ -2800,7 +2809,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>6</v>
       </c>
@@ -2823,7 +2832,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>6</v>
       </c>
@@ -2846,7 +2855,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>6</v>
       </c>
@@ -2869,7 +2878,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>6</v>
       </c>
@@ -2892,7 +2901,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>6</v>
       </c>
@@ -2915,7 +2924,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>6</v>
       </c>
@@ -2938,7 +2947,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>6</v>
       </c>
@@ -2961,7 +2970,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>6</v>
       </c>
@@ -2984,7 +2993,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>6</v>
       </c>
@@ -3007,7 +3016,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>6</v>
       </c>
@@ -3030,7 +3039,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>6</v>
       </c>
@@ -3053,7 +3062,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>6</v>
       </c>
@@ -3076,7 +3085,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>6</v>
       </c>
@@ -3099,7 +3108,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>6</v>
       </c>
@@ -3122,7 +3131,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>6</v>
       </c>
@@ -3145,7 +3154,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>6</v>
       </c>
@@ -3168,7 +3177,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>6</v>
       </c>
@@ -3191,7 +3200,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>6</v>
       </c>
@@ -3214,7 +3223,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>6</v>
       </c>
@@ -3237,7 +3246,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>6</v>
       </c>
@@ -3260,7 +3269,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>6</v>
       </c>
@@ -3283,7 +3292,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>6</v>
       </c>
@@ -3306,7 +3315,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>6</v>
       </c>
@@ -3329,7 +3338,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>6</v>
       </c>
@@ -3352,7 +3361,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>6</v>
       </c>
@@ -3375,7 +3384,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>6</v>
       </c>
@@ -3398,7 +3407,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>6</v>
       </c>
@@ -3421,7 +3430,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>6</v>
       </c>
@@ -3444,7 +3453,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>6</v>
       </c>
@@ -3467,7 +3476,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>6</v>
       </c>
@@ -3490,7 +3499,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>6</v>
       </c>
@@ -3524,9 +3533,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3552,7 +3564,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3584,11 +3596,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A1DD9D-69B1-41D9-9A06-B5167A96D339}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3608,7 +3626,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3625,7 +3643,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3642,7 +3660,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -3659,7 +3677,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -3676,7 +3694,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -3693,7 +3711,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -3710,7 +3728,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3727,7 +3745,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -3744,7 +3762,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -3761,7 +3779,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -3788,17 +3806,17 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -3812,7 +3830,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -3822,8 +3840,11 @@
       <c r="C2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -3833,8 +3854,11 @@
       <c r="C3" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>76</v>
       </c>
@@ -3843,6 +3867,9 @@
       </c>
       <c r="C4" t="s">
         <v>106</v>
+      </c>
+      <c r="D4" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -3858,18 +3885,18 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="59" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3892,7 +3919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3915,7 +3942,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3938,7 +3965,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -3961,7 +3988,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -3984,7 +4011,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -4007,7 +4034,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -4030,7 +4057,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -4053,7 +4080,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -4076,7 +4103,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -4099,7 +4126,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -4122,7 +4149,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -4145,7 +4172,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -4168,7 +4195,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -4191,7 +4218,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -4214,7 +4241,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -4237,7 +4264,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -4260,7 +4287,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -4283,7 +4310,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -4306,7 +4333,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -4329,7 +4356,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -4352,7 +4379,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -4375,7 +4402,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -4398,7 +4425,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -4421,7 +4448,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -4444,7 +4471,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -4467,7 +4494,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -4490,7 +4517,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -4513,7 +4540,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -4536,7 +4563,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -4559,7 +4586,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -4582,7 +4609,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -4605,7 +4632,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -4628,7 +4655,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -4651,7 +4678,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -4674,7 +4701,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -4697,7 +4724,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -4720,7 +4747,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -4743,7 +4770,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -4766,7 +4793,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -4789,7 +4816,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -4812,7 +4839,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -4835,7 +4862,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -4858,7 +4885,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -4881,7 +4908,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -4904,7 +4931,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>6</v>
       </c>
@@ -4927,7 +4954,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -4950,7 +4977,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -4973,7 +5000,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -4996,7 +5023,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -5019,7 +5046,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>6</v>
       </c>
@@ -5042,7 +5069,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>6</v>
       </c>
@@ -5065,7 +5092,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -5088,7 +5115,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -5111,7 +5138,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -5134,7 +5161,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -5157,7 +5184,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -5180,7 +5207,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -5203,7 +5230,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>6</v>
       </c>
@@ -5226,7 +5253,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>6</v>
       </c>
@@ -5249,7 +5276,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>6</v>
       </c>
@@ -5281,11 +5308,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BDD261B-01AD-4B96-A824-EC89AB79D98F}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5302,7 +5331,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -5316,7 +5345,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -5330,7 +5359,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -5344,7 +5373,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -5358,7 +5387,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -5372,7 +5401,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -5395,18 +5424,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F05191-328F-4CED-B8F1-6BE1926447D2}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -5420,7 +5449,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -5431,7 +5460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -5442,7 +5471,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -5453,7 +5482,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -5464,7 +5493,7 @@
         <v>9000000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -5475,7 +5504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -5486,7 +5515,7 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>78</v>
       </c>
@@ -5497,7 +5526,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -5508,7 +5537,7 @@
         <v>7000000</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -5519,7 +5548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>79</v>
       </c>
@@ -5530,7 +5559,7 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>79</v>
       </c>
@@ -5541,7 +5570,7 @@
         <v>4000000</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>79</v>
       </c>

</xml_diff>